<commit_message>
working on task base
</commit_message>
<xml_diff>
--- a/plan/excel/task_个人活动表.xlsx
+++ b/plan/excel/task_个人活动表.xlsx
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>任务ID</t>
   </si>
@@ -164,26 +164,7 @@
     <t>type</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cond</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Id</t>
-    </r>
+    <t>params</t>
   </si>
   <si>
     <t>rewards#id_cnt</t>
@@ -214,12 +195,18 @@
     <t>number</t>
   </si>
   <si>
+    <t>array</t>
+  </si>
+  <si>
     <t>map</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
+    <t>1|2|3</t>
+  </si>
+  <si>
     <t>1001_1|1002_1</t>
   </si>
   <si>
@@ -229,28 +216,13 @@
     <t>个人活动1</t>
   </si>
   <si>
+    <t>2|4|6</t>
+  </si>
+  <si>
     <t>活动标题2</t>
   </si>
   <si>
     <t>个人活动2</t>
-  </si>
-  <si>
-    <t>活动标题3</t>
-  </si>
-  <si>
-    <t>个人活动3</t>
-  </si>
-  <si>
-    <t>活动标题4</t>
-  </si>
-  <si>
-    <t>个人活动4</t>
-  </si>
-  <si>
-    <t>活动标题5</t>
-  </si>
-  <si>
-    <t>个人活动5</t>
   </si>
 </sst>
 </file>
@@ -258,12 +230,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,10 +244,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -287,7 +260,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,61 +288,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -376,69 +317,82 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -451,6 +405,17 @@
       <name val="Tahoma"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -461,13 +426,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,7 +552,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,6 +570,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -503,145 +606,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,6 +617,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -666,17 +655,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -699,8 +677,28 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -719,49 +717,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -770,16 +735,16 @@
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -788,123 +753,122 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1256,13 +1220,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="7.5" customWidth="1"/>
     <col min="2" max="2" width="12.875" customWidth="1"/>
@@ -1282,7 +1246,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -1296,16 +1260,16 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1319,16 +1283,16 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -1345,28 +1309,28 @@
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>1001</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>3600</v>
@@ -1374,109 +1338,40 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>1002</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>3600</v>
+        <v>86400</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="1">
-        <v>1</v>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>1003</v>
-      </c>
-      <c r="B7">
-        <v>3600</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>1004</v>
-      </c>
-      <c r="B8">
-        <v>3600</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>1005</v>
-      </c>
-      <c r="B9">
-        <v>86400</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>